<commit_message>
Flesh out possible implementation
</commit_message>
<xml_diff>
--- a/src/datafev/algorithms/reinforcement_learning/geolocation/inputs/example_01.xlsx
+++ b/src/datafev/algorithms/reinforcement_learning/geolocation/inputs/example_01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gelsaine_L\Documents\Pycharm Projects\datafev\src\datafev\algorithms\geolocation\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a05a06f3caea666/Documents/GitHub/datafev/src/datafev/algorithms/reinforcement_learning/geolocation/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C08CCBB-34B6-483F-A77F-002E8EC3C5AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{8C08CCBB-34B6-483F-A77F-002E8EC3C5AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FF96393-3F28-4B44-BDEA-80B81ABBCB92}"/>
   <bookViews>
-    <workbookView xWindow="38610" yWindow="0" windowWidth="38190" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation" sheetId="6" r:id="rId1"/>
@@ -154,9 +154,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -194,9 +194,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -229,9 +229,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -264,9 +281,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -443,16 +477,16 @@
   <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -523,15 +557,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44569.291666261583</v>
       </c>
       <c r="B2">
-        <v>42.9890408359568</v>
+        <v>42.989040840000001</v>
       </c>
       <c r="C2">
-        <v>-81.228214933944599</v>
+        <v>-81.228214929999993</v>
       </c>
       <c r="D2">
         <v>42.985230414809799</v>
@@ -594,15 +628,15 @@
         <v>-81.247673979428697</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44569.302083333336</v>
       </c>
       <c r="B3">
-        <v>42.9858738421377</v>
+        <v>42.986799697825198</v>
       </c>
       <c r="C3">
-        <v>-81.236837318590204</v>
+        <v>-81.227937513089998</v>
       </c>
       <c r="D3">
         <v>42.985230414809799</v>
@@ -665,15 +699,15 @@
         <v>-81.247673979428697</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44569.3125</v>
       </c>
       <c r="B4">
-        <v>42.984881769885099</v>
+        <v>42.986657532755402</v>
       </c>
       <c r="C4">
-        <v>-81.250959123144398</v>
+        <v>-81.230996674159698</v>
       </c>
       <c r="D4">
         <v>42.985230414809799</v>
@@ -736,15 +770,15 @@
         <v>-81.247673979428697</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>44569.322916666664</v>
       </c>
       <c r="B5">
-        <v>42.988375518508199</v>
+        <v>42.984427370468701</v>
       </c>
       <c r="C5">
-        <v>-81.254614872268107</v>
+        <v>-81.230586739052399</v>
       </c>
       <c r="D5">
         <v>42.985230414809799</v>
@@ -807,15 +841,15 @@
         <v>-81.247673979428697</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>44569.333333333336</v>
       </c>
       <c r="B6">
-        <v>42.993011977016501</v>
+        <v>42.984427370468701</v>
       </c>
       <c r="C6">
-        <v>-81.256767047192199</v>
+        <v>-81.230586739052399</v>
       </c>
       <c r="D6">
         <v>42.985230414809799</v>
@@ -878,15 +912,15 @@
         <v>-81.247673979428697</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>44569.34375</v>
       </c>
       <c r="B7">
-        <v>42.991240512172503</v>
+        <v>42.984427370468701</v>
       </c>
       <c r="C7">
-        <v>-81.267828502447102</v>
+        <v>-81.230586739052399</v>
       </c>
       <c r="D7">
         <v>42.985230414809799</v>
@@ -949,15 +983,15 @@
         <v>-81.247673979428697</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>44569.354166666664</v>
       </c>
       <c r="B8">
-        <v>42.986819583258203</v>
+        <v>42.984427370468701</v>
       </c>
       <c r="C8">
-        <v>-81.282598907559404</v>
+        <v>-81.230586739052399</v>
       </c>
       <c r="D8">
         <v>42.985230414809799</v>
@@ -1020,15 +1054,15 @@
         <v>-81.247673979428697</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>44569.364583333336</v>
       </c>
       <c r="B9">
-        <v>42.983757094862902</v>
+        <v>42.984395306414903</v>
       </c>
       <c r="C9">
-        <v>-81.293241854258198</v>
+        <v>-81.233651596635298</v>
       </c>
       <c r="D9">
         <v>42.985230414809799</v>
@@ -1091,7 +1125,7 @@
         <v>-81.247673979428697</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
     </row>
   </sheetData>

</xml_diff>